<commit_message>
Reducing number of components.
- removing 9-12v power supply option;
- replacing 74hc14 with 74hc540;
</commit_message>
<xml_diff>
--- a/midi_splitter-bom.xlsx
+++ b/midi_splitter-bom.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max_romanov/projects/midi_splitter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED25C8A-E63E-1F4B-89BF-A277D2D73FB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671E89C1-6579-0341-AD36-FB1C6EAACB5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="960" windowWidth="27240" windowHeight="16540" activeTab="1" xr2:uid="{A1306BC4-A011-3F4B-B468-299FA49377F1}"/>
+    <workbookView xWindow="1180" yWindow="960" windowWidth="27240" windowHeight="16540" activeTab="2" xr2:uid="{A1306BC4-A011-3F4B-B468-299FA49377F1}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM" sheetId="1" r:id="rId1"/>
-    <sheet name="Orders" sheetId="2" r:id="rId2"/>
+    <sheet name="x6" sheetId="1" r:id="rId1"/>
+    <sheet name="x6-2" sheetId="3" r:id="rId2"/>
+    <sheet name="Orders" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="183">
   <si>
     <t>id</t>
   </si>
@@ -482,6 +483,99 @@
   </si>
   <si>
     <t>L-KLS1-DC-005A-2.0</t>
+  </si>
+  <si>
+    <t>C1,C2</t>
+  </si>
+  <si>
+    <t>R14,R16</t>
+  </si>
+  <si>
+    <t>1n914</t>
+  </si>
+  <si>
+    <t>mm74hc540mtcx</t>
+  </si>
+  <si>
+    <t>TSSOP-20</t>
+  </si>
+  <si>
+    <t>MM74HC540MTCX</t>
+  </si>
+  <si>
+    <t>Восемь буферных элементов, драйверов с тремя состояниями на выходе</t>
+  </si>
+  <si>
+    <t>#1517354</t>
+  </si>
+  <si>
+    <t>Rezonit</t>
+  </si>
+  <si>
+    <t>#564131</t>
+  </si>
+  <si>
+    <t>#251110</t>
+  </si>
+  <si>
+    <t>CC0805KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>L-13GD</t>
+  </si>
+  <si>
+    <t>Светодиод Flat Top зеленый 70° d=2мм 10мКд 568нМ</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>#307856</t>
+  </si>
+  <si>
+    <t>Flat Top красный</t>
+  </si>
+  <si>
+    <t>#3638121</t>
+  </si>
+  <si>
+    <t>#4000903717748</t>
+  </si>
+  <si>
+    <t>#32874392571</t>
+  </si>
+  <si>
+    <t>#1005002547515126</t>
+  </si>
+  <si>
+    <t>#5017461801272510</t>
+  </si>
+  <si>
+    <t>#07863451</t>
+  </si>
+  <si>
+    <t>#8341083</t>
+  </si>
+  <si>
+    <t>#5017385647722510</t>
+  </si>
+  <si>
+    <t>#8338098</t>
+  </si>
+  <si>
+    <t>#8341104</t>
+  </si>
+  <si>
+    <t>rezonit.ru</t>
+  </si>
+  <si>
+    <t>chipdip.ru</t>
+  </si>
+  <si>
+    <t>L-13ID</t>
   </si>
 </sst>
 </file>
@@ -492,7 +586,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ _R_U_B"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -510,8 +604,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,8 +632,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -631,12 +739,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -738,6 +857,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -747,12 +884,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -760,6 +923,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF2F2F2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1071,7 +1239,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1092,41 +1260,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="55" t="s">
+      <c r="G1" s="62"/>
+      <c r="H1" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="59"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="65"/>
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1194,13 +1362,13 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="59" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="8">
         <v>0</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="60" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="41" t="s">
@@ -1234,11 +1402,11 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="60"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="8">
         <v>1</v>
       </c>
-      <c r="C5" s="61"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="52" t="s">
         <v>149</v>
       </c>
@@ -2179,11 +2347,792 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FAADAA-4ED6-1B47-9ADF-86E276BEC7B9}">
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="62"/>
+      <c r="H1" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="16">
+        <v>44642</v>
+      </c>
+      <c r="J3" s="24">
+        <v>224</v>
+      </c>
+      <c r="K3" s="13">
+        <v>21</v>
+      </c>
+      <c r="L3" s="24"/>
+      <c r="M3" s="22">
+        <f t="shared" ref="M3:M17" si="0">J3*K3+L3</f>
+        <v>4704</v>
+      </c>
+      <c r="N3" s="25">
+        <f t="shared" ref="N3:N17" si="1">M3/K3*B3</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I4" s="11">
+        <v>44642</v>
+      </c>
+      <c r="J4" s="23">
+        <v>14</v>
+      </c>
+      <c r="K4" s="8">
+        <v>20</v>
+      </c>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="N4" s="26">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="I5" s="16">
+        <v>44625</v>
+      </c>
+      <c r="J5" s="24">
+        <f>355.04/K5</f>
+        <v>17.752000000000002</v>
+      </c>
+      <c r="K5" s="13">
+        <v>20</v>
+      </c>
+      <c r="L5" s="24">
+        <v>99.52</v>
+      </c>
+      <c r="M5" s="24">
+        <f t="shared" si="0"/>
+        <v>454.56000000000006</v>
+      </c>
+      <c r="N5" s="27">
+        <f t="shared" si="1"/>
+        <v>22.728000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I6" s="11">
+        <v>44641</v>
+      </c>
+      <c r="J6" s="23">
+        <v>26</v>
+      </c>
+      <c r="K6" s="8">
+        <v>21</v>
+      </c>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23">
+        <f t="shared" si="0"/>
+        <v>546</v>
+      </c>
+      <c r="N6" s="26">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="13">
+        <v>7</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="I7" s="16">
+        <v>44634</v>
+      </c>
+      <c r="J7" s="24">
+        <f>6604.81/K7</f>
+        <v>22.016033333333336</v>
+      </c>
+      <c r="K7" s="13">
+        <v>300</v>
+      </c>
+      <c r="L7" s="24">
+        <v>1711.62</v>
+      </c>
+      <c r="M7" s="24">
+        <f t="shared" si="0"/>
+        <v>8316.43</v>
+      </c>
+      <c r="N7" s="27">
+        <f t="shared" si="1"/>
+        <v>194.05003333333335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="I8" s="11">
+        <v>44642</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="8">
+        <v>20</v>
+      </c>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23">
+        <v>7624.08</v>
+      </c>
+      <c r="N8" s="26">
+        <f t="shared" si="1"/>
+        <v>381.20400000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="13">
+        <v>13</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="I9" s="16">
+        <v>44642</v>
+      </c>
+      <c r="J9" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="K9" s="13">
+        <v>800</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="N9" s="27">
+        <f t="shared" si="1"/>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="I10" s="16">
+        <v>44642</v>
+      </c>
+      <c r="J10" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="K10" s="8">
+        <v>400</v>
+      </c>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="N10" s="26">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="I11" s="16">
+        <v>44642</v>
+      </c>
+      <c r="J11" s="24">
+        <v>0.32</v>
+      </c>
+      <c r="K11" s="13">
+        <v>100</v>
+      </c>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="N11" s="27">
+        <f t="shared" si="1"/>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="8">
+        <v>2</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="I12" s="16">
+        <v>44642</v>
+      </c>
+      <c r="J12" s="23">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K12" s="8">
+        <v>30</v>
+      </c>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+      <c r="N12" s="26">
+        <f t="shared" si="1"/>
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="I13" s="16">
+        <v>44642</v>
+      </c>
+      <c r="J13" s="24">
+        <v>0.66</v>
+      </c>
+      <c r="K13" s="13">
+        <v>400</v>
+      </c>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24">
+        <f t="shared" si="0"/>
+        <v>264</v>
+      </c>
+      <c r="N13" s="27">
+        <f t="shared" si="1"/>
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="71" t="s">
+        <v>165</v>
+      </c>
+      <c r="B14" s="72">
+        <v>1</v>
+      </c>
+      <c r="C14" s="73" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" s="73" t="s">
+        <v>166</v>
+      </c>
+      <c r="E14" s="74"/>
+      <c r="F14" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76" t="s">
+        <v>179</v>
+      </c>
+      <c r="I14" s="77">
+        <v>44642</v>
+      </c>
+      <c r="J14" s="78">
+        <v>29</v>
+      </c>
+      <c r="K14" s="72">
+        <v>70</v>
+      </c>
+      <c r="L14" s="78"/>
+      <c r="M14" s="79">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="N14" s="80">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" s="13">
+        <v>1</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="67"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="I15" s="16">
+        <v>44642</v>
+      </c>
+      <c r="J15" s="70">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K15" s="13">
+        <v>3</v>
+      </c>
+      <c r="L15" s="70"/>
+      <c r="M15" s="24">
+        <f t="shared" si="0"/>
+        <v>29.400000000000002</v>
+      </c>
+      <c r="N15" s="27">
+        <f t="shared" si="1"/>
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="I16" s="16">
+        <v>44642</v>
+      </c>
+      <c r="J16" s="23">
+        <v>11.3</v>
+      </c>
+      <c r="K16" s="8">
+        <v>40</v>
+      </c>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23">
+        <f>J16*K16+L16</f>
+        <v>452</v>
+      </c>
+      <c r="N16" s="26">
+        <f>M16/K16*B16</f>
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="29">
+        <v>1</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1812</v>
+      </c>
+      <c r="F17" s="30"/>
+      <c r="G17" s="51" t="s">
+        <v>171</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="2">
+        <v>44642</v>
+      </c>
+      <c r="J17" s="28">
+        <f>582.63/K17</f>
+        <v>9.7104999999999997</v>
+      </c>
+      <c r="K17" s="29">
+        <v>60</v>
+      </c>
+      <c r="L17" s="28">
+        <v>245.58</v>
+      </c>
+      <c r="M17" s="24">
+        <f t="shared" si="0"/>
+        <v>828.21</v>
+      </c>
+      <c r="N17" s="27">
+        <f t="shared" si="1"/>
+        <v>13.803500000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="L18" s="28">
+        <f>SUM(L3:L17)</f>
+        <v>2056.7199999999998</v>
+      </c>
+      <c r="M18" s="28">
+        <f>SUM(M3:M17)</f>
+        <v>25869.08</v>
+      </c>
+      <c r="N18" s="28">
+        <f>SUM(N3:N17)</f>
+        <v>931.58553333333339</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{7592010A-2839-C542-A68C-36B429A3F9E6}"/>
+    <hyperlink ref="F13" r:id="rId2" xr:uid="{E8F78C2F-9B2F-F34B-8F0A-F0DE0F8892E4}"/>
+    <hyperlink ref="F12" r:id="rId3" xr:uid="{007969DC-82B9-0D42-BB4A-C47A061181AF}"/>
+    <hyperlink ref="F11" r:id="rId4" xr:uid="{2F6B5033-470A-634F-B48F-89129456372D}"/>
+    <hyperlink ref="F9" r:id="rId5" xr:uid="{3FD2808F-E81E-7C43-9123-EA1CF3D01AA9}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{3E936503-C830-DD40-9D5E-FF803B685AD8}"/>
+    <hyperlink ref="G16" r:id="rId7" xr:uid="{8209FFA3-6A3A-F947-B81D-56F966FB4B01}"/>
+    <hyperlink ref="G3" r:id="rId8" display="60026" xr:uid="{8CF3F62A-B870-EF47-A50B-24EBC51B30F1}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{7E7EB2DE-CDD6-2244-AB7C-2AE7CE204583}"/>
+    <hyperlink ref="G11" r:id="rId10" xr:uid="{E1475508-387A-814D-B097-F8ADA07A31D9}"/>
+    <hyperlink ref="G12" r:id="rId11" xr:uid="{6828B6EA-4193-284A-9C34-01363272634C}"/>
+    <hyperlink ref="G13" r:id="rId12" xr:uid="{DFF35B3A-492E-774B-9C22-B3B0F2E31139}"/>
+    <hyperlink ref="F4" r:id="rId13" xr:uid="{3F21A7B8-3ACF-AF42-9A9D-0AA4F57E7802}"/>
+    <hyperlink ref="F6" r:id="rId14" display="https://www.chipdip.ru/product/mm74hc540mtcx" xr:uid="{BACB03E8-DF15-EC48-9253-E43577DBAF0F}"/>
+    <hyperlink ref="G9" r:id="rId15" xr:uid="{916D04E9-148A-7A42-86D7-557B74784CDB}"/>
+    <hyperlink ref="F14" r:id="rId16" xr:uid="{ED837917-924D-1840-9B5F-E0C10F148C1A}"/>
+    <hyperlink ref="G15" r:id="rId17" xr:uid="{6577E776-FEB7-A847-BB6F-41363D533E4F}"/>
+    <hyperlink ref="G5" r:id="rId18" xr:uid="{1AABE177-007B-3C46-9DEB-15E464962369}"/>
+    <hyperlink ref="G7" r:id="rId19" xr:uid="{4FB16798-FF7D-4649-B3B7-1E51E9D9FF48}"/>
+    <hyperlink ref="H7" r:id="rId20" xr:uid="{2F6E14C1-9827-6F4B-9B95-E025B2332F01}"/>
+    <hyperlink ref="H8" r:id="rId21" xr:uid="{F35AE100-86A0-DB47-A05F-F1C1D0D98627}"/>
+    <hyperlink ref="H3" r:id="rId22" xr:uid="{8F8DC0E8-B428-5245-BF6E-A364D12EFC57}"/>
+    <hyperlink ref="H4" r:id="rId23" xr:uid="{C4809539-778C-604D-823A-7DA5D42F224E}"/>
+    <hyperlink ref="H5" r:id="rId24" xr:uid="{95735363-6864-3C4C-90EC-9B56D60A568B}"/>
+    <hyperlink ref="H6" r:id="rId25" xr:uid="{3F755EEE-AFF3-924C-9DAB-5F703EFB75F3}"/>
+    <hyperlink ref="H9" r:id="rId26" xr:uid="{749C49C4-A5DD-8E4C-961A-76CD2609BCF6}"/>
+    <hyperlink ref="H10" r:id="rId27" xr:uid="{010946ED-9FFD-8446-8811-EF3F6434DD01}"/>
+    <hyperlink ref="H11" r:id="rId28" xr:uid="{539ECBEA-FEDD-7B4D-9F52-98102B508A03}"/>
+    <hyperlink ref="H12" r:id="rId29" xr:uid="{1ECB32E6-296B-7F41-A817-94F42EEEF76D}"/>
+    <hyperlink ref="H13" r:id="rId30" xr:uid="{E5414779-9D09-9C49-8B14-C8D589641AD7}"/>
+    <hyperlink ref="H15" r:id="rId31" xr:uid="{6A53B4A2-CE20-C742-B4C6-ED420DBF8F40}"/>
+    <hyperlink ref="H16" r:id="rId32" xr:uid="{D9490399-74C5-CA43-A5CF-DBB8AB039CF0}"/>
+    <hyperlink ref="H14" r:id="rId33" xr:uid="{3C14CFA5-029B-BA47-A7AC-FDDE3FA35FB5}"/>
+    <hyperlink ref="G17" r:id="rId34" xr:uid="{E7D8D255-CB26-8144-8E25-46F25720CDBA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEE308A-D149-EF40-BE09-A34256E797F5}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2581,7 +3530,199 @@
         <v>3807.23</v>
       </c>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="42">
+        <v>44625</v>
+      </c>
+      <c r="E20" s="82" t="s">
+        <v>177</v>
+      </c>
+      <c r="F20">
+        <v>355.04</v>
+      </c>
+      <c r="G20">
+        <v>99.52</v>
+      </c>
+      <c r="H20">
+        <f>F20+G20</f>
+        <v>454.56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21">
+        <v>300</v>
+      </c>
+      <c r="C21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="42">
+        <v>44634</v>
+      </c>
+      <c r="E21" s="82" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21">
+        <v>6604.81</v>
+      </c>
+      <c r="G21">
+        <v>1711.62</v>
+      </c>
+      <c r="H21">
+        <f>F21+G21</f>
+        <v>8316.43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>181</v>
+      </c>
+      <c r="D22" s="42">
+        <v>44641</v>
+      </c>
+      <c r="E22" s="81" t="s">
+        <v>178</v>
+      </c>
+      <c r="F22">
+        <v>651</v>
+      </c>
+      <c r="H22">
+        <f>F22+G22</f>
+        <v>651</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>180</v>
+      </c>
+      <c r="D23" s="42">
+        <v>44642</v>
+      </c>
+      <c r="E23" s="81" t="s">
+        <v>159</v>
+      </c>
+      <c r="H23">
+        <v>7624.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="85"/>
+      <c r="C24" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" s="42">
+        <v>44642</v>
+      </c>
+      <c r="E24" s="81" t="s">
+        <v>176</v>
+      </c>
+      <c r="F24">
+        <v>4430</v>
+      </c>
+      <c r="H24">
+        <f>F24+G24</f>
+        <v>4430</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="42">
+        <v>44642</v>
+      </c>
+      <c r="E25" s="82" t="s">
+        <v>175</v>
+      </c>
+      <c r="F25">
+        <v>10778.4</v>
+      </c>
+      <c r="G25">
+        <v>236</v>
+      </c>
+      <c r="H25">
+        <f>F25+G25</f>
+        <v>11014.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="84" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
+        <v>181</v>
+      </c>
+      <c r="D26" s="42">
+        <v>44642</v>
+      </c>
+      <c r="E26" s="83" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26">
+        <v>2030</v>
+      </c>
+      <c r="H26">
+        <f>F26+G26</f>
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="42">
+        <v>44642</v>
+      </c>
+      <c r="E27" s="51" t="s">
+        <v>171</v>
+      </c>
+      <c r="F27">
+        <v>582.63</v>
+      </c>
+      <c r="G27">
+        <v>245.58</v>
+      </c>
+      <c r="H27">
+        <f>F27+G27</f>
+        <v>828.21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H28">
+        <f>SUM(H20:H27)</f>
+        <v>35348.68</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A20:H27">
+    <sortCondition ref="D20:D27"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{D550EA50-9C44-A443-90F2-FDA717C60B8A}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{9AF8BA5C-986A-9F40-933A-5891D237766F}"/>
@@ -2592,6 +3733,14 @@
     <hyperlink ref="E15" r:id="rId7" xr:uid="{7541DEB4-F288-8B46-A39C-23C6A08145E8}"/>
     <hyperlink ref="E16" r:id="rId8" xr:uid="{9915FBE3-0302-624D-91CC-FE7815A2D03D}"/>
     <hyperlink ref="E17" r:id="rId9" xr:uid="{143F4188-41FE-FB4D-8D15-C3786255948E}"/>
+    <hyperlink ref="E23" r:id="rId10" display="https://service.rezonit.ru/orders/1168288" xr:uid="{B7703450-7663-DC4B-B792-F4CDB43C1D13}"/>
+    <hyperlink ref="E20" r:id="rId11" display="https://trade.aliexpress.ru/order_detail.htm?spm=a2g39.orderlist.0.0.43064aa6aMZspA&amp;orderId=5017385647722510&amp;orderSource=GlobalTrade" xr:uid="{D1E2FF23-C973-9544-A4BA-822EE2012243}"/>
+    <hyperlink ref="E22" r:id="rId12" display="https://www.chipdip.ru/order/detail/8338098" xr:uid="{EA91DE6B-FF6C-1243-84D9-8D68AB65604A}"/>
+    <hyperlink ref="E21" r:id="rId13" display="https://trade.aliexpress.ru/order_detail.htm?spm=a2g39.orderlist.0.0.43064aa6aMZspA&amp;orderId=5017461801272510&amp;orderSource=GlobalTrade" xr:uid="{92D5B84E-6A32-944E-8290-157A16F41C6A}"/>
+    <hyperlink ref="E25" r:id="rId14" display="https://www.terraelectronica.ru/order/07863451" xr:uid="{D2BCC303-8E71-2544-936A-3955C9B05A93}"/>
+    <hyperlink ref="E26" r:id="rId15" display="https://www.chipdip.ru/order/detail/8341104" xr:uid="{5990DDED-7BC1-EB46-940B-C395749F80D2}"/>
+    <hyperlink ref="E27" r:id="rId16" display="https://www.aliexpress.ru/item/4000903717748.html" xr:uid="{83E0D37B-0463-0E4E-90C4-68A8F7FE34EB}"/>
+    <hyperlink ref="E24" r:id="rId17" display="https://www.chipdip.ru/order/detail/8341083" xr:uid="{6D105DFB-EB00-2B41-8929-2D48FD3A004C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>